<commit_message>
Run linter for Vercel
</commit_message>
<xml_diff>
--- a/public/tempEntrada.xlsx
+++ b/public/tempEntrada.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>D.G.C.F.T</t>
   </si>
@@ -34,7 +34,7 @@
     <t>FACTURA NÚM:</t>
   </si>
   <si>
-    <t>A21216406</t>
+    <t>A21216407</t>
   </si>
   <si>
     <t>DIA</t>
@@ -58,7 +58,7 @@
     <t>NÚMERO</t>
   </si>
   <si>
-    <t>Oxxo</t>
+    <t>Office Depot</t>
   </si>
   <si>
     <t>PARTIDA</t>
@@ -82,25 +82,13 @@
     <t>OBSERVACIONES</t>
   </si>
   <si>
-    <t>21101 - Materiales y útiles de oficina</t>
-  </si>
-  <si>
-    <t>Caja de Lapices</t>
+    <t>21101</t>
+  </si>
+  <si>
+    <t>Caja de papel bond</t>
   </si>
   <si>
     <t>Caja</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>3400 - Servicios financieros, bancarios y comerciales</t>
-  </si>
-  <si>
-    <t>Tarjeta de crédito escolar</t>
-  </si>
-  <si>
-    <t>Pieza</t>
   </si>
   <si>
     <t>Ninguna</t>
@@ -752,7 +740,7 @@
         <v>13</v>
       </c>
       <c r="F6" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="9" t="s">
@@ -809,13 +797,13 @@
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="13">
-        <v>45</v>
+        <v>350</v>
       </c>
       <c r="I9" s="13">
         <f>F9 * H9</f>
@@ -827,31 +815,19 @@
       <c r="K9" s="11"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>27</v>
-      </c>
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
-      <c r="F10" s="11">
-        <v>1</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="13">
-        <v>0</v>
-      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13"/>
       <c r="I10" s="13">
         <f t="shared" ref="I10:I22" si="0">F10 * H10</f>
         <v>0</v>
       </c>
-      <c r="J10" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="J10" s="11"/>
       <c r="K10" s="11"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1067,57 +1043,57 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="E25" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="I25" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C26" s="11"/>
       <c r="E26" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G26" s="11"/>
       <c r="I26" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J26" s="11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K26" s="11"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
       <c r="E27" s="14" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
       <c r="I27" s="14" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="J27" s="14"/>
       <c r="K27" s="14"/>

</xml_diff>

<commit_message>
Modulo de salida completado
</commit_message>
<xml_diff>
--- a/public/tempEntrada.xlsx
+++ b/public/tempEntrada.xlsx
@@ -22,7 +22,7 @@
     <t>CENTRO DE CAPACITACIÓN PARA EL TRABAJO INDUSTRIAL NO. 50</t>
   </si>
   <si>
-    <t>12</t>
+    <t>13</t>
   </si>
   <si>
     <t>07</t>
@@ -58,7 +58,7 @@
     <t>NÚMERO</t>
   </si>
   <si>
-    <t>Office Depot</t>
+    <t>SuperTony Papeleria</t>
   </si>
   <si>
     <t>PARTIDA</t>
@@ -82,13 +82,13 @@
     <t>OBSERVACIONES</t>
   </si>
   <si>
-    <t>21101</t>
-  </si>
-  <si>
-    <t>Caja de papel bond</t>
-  </si>
-  <si>
-    <t>Caja</t>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>Silla de escritorio</t>
+  </si>
+  <si>
+    <t>Pieza</t>
   </si>
   <si>
     <t>Ninguna</t>
@@ -740,7 +740,7 @@
         <v>13</v>
       </c>
       <c r="F6" s="7">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="9" t="s">
@@ -803,7 +803,7 @@
         <v>24</v>
       </c>
       <c r="H9" s="13">
-        <v>350</v>
+        <v>100</v>
       </c>
       <c r="I9" s="13">
         <f>F9 * H9</f>

</xml_diff>

<commit_message>
Modulo de existencias completado
</commit_message>
<xml_diff>
--- a/public/tempEntrada.xlsx
+++ b/public/tempEntrada.xlsx
@@ -22,7 +22,7 @@
     <t>CENTRO DE CAPACITACIÓN PARA EL TRABAJO INDUSTRIAL NO. 50</t>
   </si>
   <si>
-    <t>13</t>
+    <t>19</t>
   </si>
   <si>
     <t>07</t>
@@ -34,7 +34,7 @@
     <t>FACTURA NÚM:</t>
   </si>
   <si>
-    <t>A21216407</t>
+    <t>A21216406</t>
   </si>
   <si>
     <t>DIA</t>
@@ -58,7 +58,7 @@
     <t>NÚMERO</t>
   </si>
   <si>
-    <t>SuperTony Papeleria</t>
+    <t>Office Depot</t>
   </si>
   <si>
     <t>PARTIDA</t>
@@ -82,10 +82,10 @@
     <t>OBSERVACIONES</t>
   </si>
   <si>
-    <t>5000</t>
-  </si>
-  <si>
-    <t>Silla de escritorio</t>
+    <t>21201</t>
+  </si>
+  <si>
+    <t>Tinta de impresora marca Epson</t>
   </si>
   <si>
     <t>Pieza</t>
@@ -106,7 +106,7 @@
     <t>NOMBRE</t>
   </si>
   <si>
-    <t>Tila del Carmen Mendoza Olán</t>
+    <t>Tila del Carmen Mendoza Olan</t>
   </si>
   <si>
     <t>Abraham Espinosa Mendoza</t>
@@ -740,7 +740,7 @@
         <v>13</v>
       </c>
       <c r="F6" s="7">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="9" t="s">
@@ -797,13 +797,13 @@
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="13">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="I9" s="13">
         <f>F9 * H9</f>

</xml_diff>